<commit_message>
File updates on program run
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,44 @@
           <t>notes</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45912.28803851852</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>45912.28803851852</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45912.28809836806</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -511,7 +549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,10 +642,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>45912.28862107639</v>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
     </row>
@@ -639,10 +679,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>45912.28908845241</v>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
     </row>
@@ -698,23 +740,23 @@
           <t>ਚੰਦਨ ਅਗਰ ਕਪੂਰ ਲੇਪਨ ਤਿਸੁ ਸੰਗੇ ਨਹੀ ਪ੍ਰੀਤਿ ॥</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1018</t>
-        </is>
+      <c r="E5" t="n">
+        <v>1018</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45912.27207551573</v>
+        <v>45912.27207552084</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>45912.28862107639</v>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
     </row>
@@ -735,23 +777,23 @@
           <t>ਜਟਾ ਭਸਮ ਲੇਪਨ ਕੀਆ ਕਹਾ ਗੁਫਾ ਮਹਿ ਬਾਸੁ ॥</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1103</t>
-        </is>
+      <c r="E6" t="n">
+        <v>1103</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45912.27207551573</v>
+        <v>45912.27207552084</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>45912.28908845241</v>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
     </row>
@@ -772,16 +814,14 @@
           <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1243</t>
-        </is>
+      <c r="E7" t="n">
+        <v>1243</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45912.27207551573</v>
+        <v>45912.27207552084</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -791,6 +831,115 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ਚੰਦਨ ਅਗਰ ਕਪੂਰ ਲੇਪਨ ਤਿਸੁ ਸੰਗੇ ਨਹੀ ਪ੍ਰੀਤਿ ॥</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1018</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>45912.28803851852</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>45912.28862107639</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ਜਟਾ ਭਸਮ ਲੇਪਨ ਕੀਆ ਕਹਾ ਗੁਫਾ ਮਹਿ ਬਾਸੁ ॥</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>1103</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>45912.28803851852</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>45912.28908845241</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>45912.28803851852</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update on programm run output files
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -549,7 +549,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="I3" s="2" t="n">
-        <v>45912.28908845241</v>
+        <v>45912.28908844908</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="I6" s="2" t="n">
-        <v>45912.28908845241</v>
+        <v>45912.28908844908</v>
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="I9" s="2" t="n">
-        <v>45912.28908845241</v>
+        <v>45912.28908844908</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -940,6 +940,216 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ਚੰਦਨ ਅਗਰ ਕਪੂਰ ਲੇਪਨ ਤਿਸੁ ਸੰਗੇ ਨਹੀ ਪ੍ਰੀਤਿ ॥</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>1018</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>45912.30713481482</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ਜਟਾ ਭਸਮ ਲੇਪਨ ਕੀਆ ਕਹਾ ਗੁਫਾ ਮਹਿ ਬਾਸੁ ॥</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1103</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>45912.30713481482</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>45912.30713481482</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ਚੰਦਨ ਅਗਰ ਕਪੂਰ ਲੇਪਨ ਤਿਸੁ ਸੰਗੇ ਨਹੀ ਪ੍ਰੀਤਿ ॥</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>1018</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>45912.31589575231</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ਜਟਾ ਭਸਮ ਲੇਪਨ ਕੀਆ ਕਹਾ ਗੁਫਾ ਮਹਿ ਬਾਸੁ ॥</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>1103</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>45912.31589575231</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>45912.31589575231</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(assess-by-word): dedicated analyzer window with integrated driver controls; launch from driver; tracker updates and taskbar-safe UI; add screenshots
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -587,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -770,6 +770,111 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ਚੰਦਨ ਅਗਰ ਕਪੂਰ ਲੇਪਨ ਤਿਸੁ ਸੰਗੇ ਨਹੀ ਪ੍ਰੀਤਿ ॥</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1018</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>45914.24793988426</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ਜਟਾ ਭਸਮ ਲੇਪਨ ਕੀਆ ਕਹਾ ਗੁਫਾ ਮਹਿ ਬਾਸੁ ॥</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>1103</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>45914.24793988426</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ਲੇਪਨ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>45914.24793988426</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix(abw): restore full translation input UI; stop out-of-scope refs; add smoke script and before/after screenshots (root cause: mis-indented early return)
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -576,6 +576,44 @@
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>45914.27813299769</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>45914.27813299769</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>45914.27817406424</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -587,7 +625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -875,6 +913,111 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ਮਨਮੁਖ ਦੁਬਿਧਾ ਦੁਰਮਤਿ ਬਿਆਪੇ ਜਿਨ ਅੰਤਰਿ ਮੋਹ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>507</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>45914.27813299769</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ਜਿਨ੍ਹ੍ਹਿ ਕੀਏ ਤਿਸਹਿ ਨ ਜਾਣਨੀ ਮਨਮੁਖਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>788</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>45914.27813299769</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>45914.27813299769</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(abw): finish ABW separation; use dedicated analyzer + submission flow; gate old driver controller; add _strip_terminators and test; fix danda/punctuation tokenization
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>45914.27817406424</v>
+        <v>45914.2781740625</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -625,7 +625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -1018,6 +1018,111 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ਮਨਮੁਖ ਦੁਬਿਧਾ ਦੁਰਮਤਿ ਬਿਆਪੇ ਜਿਨ ਅੰਤਰਿ ਮੋਹ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>507</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>45914.29202659722</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ਜਿਨ੍ਹ੍ਹਿ ਕੀਏ ਤਿਸਹਿ ਨ ਜਾਣਨੀ ਮਨਮੁਖਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>788</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>45914.29202659722</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>45914.29202659722</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated output file for assessment by word
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -576,6 +576,44 @@
       </c>
       <c r="L2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>45914.46202929398</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>45914.46202929398</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>45914.46206456018</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -587,7 +625,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -770,6 +808,111 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ਮਨਮੁਖ ਦੁਬਿਧਾ ਦੁਰਮਤਿ ਬਿਆਪੇ ਜਿਨ ਅੰਤਰਿ ਮੋਹ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>507</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>45914.46202929398</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ਜਿਨ੍ਹ੍ਹਿ ਕੀਏ ਤਿਸਹਿ ਨ ਜਾਣਨੀ ਮਨਮੁਖਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>788</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>45914.46202929398</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ਗੁਬਾਰੀ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ਬਾਹਰਿ ਭਸਮ ਲੇਪਨ ਕਰੇ ਅੰਤਰਿ ਗੁਬਾਰੀ ॥</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1243</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>45914.46202929398</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Output file updates ## Context
## Objective

## KEEP

## IMPROVE #1
- Severity (P1/P2/P3):
- Rationale:
- Codex, please ...
- Acceptance criteria:
  - [ ]

<!-- Repeat IMPROVE block as needed -->

## Global checks
- [ ] Definition of Done
- [ ] No P1/P2
- [ ] No regressions
- [ ] Stability Guards
- [ ] Idempotency
- [ ] Verification evidence attached
- [ ] Ready to CONVERGE

## Assumptions (optional)

## Verification
<!-- Minimal evidence:
make qa-fast
python -m py_compile 1.1.0_birha.py
# attach screenshot/output for acceptance criteria -->

## Exit
<!-- write "CONVERGED" if done, and list any low-value optimizations intentionally deferred -->
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A2:XFD3"/>
@@ -618,6 +618,44 @@
       </c>
       <c r="L3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>45916.27149407408</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -629,7 +667,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A2:XFD7"/>
@@ -892,6 +930,3475 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਰੇ ਮਨ ਚਿਤਵਹਿ ਉਦਮੁ ਜਾ ਆਹਰਿ ਹਰਿ ਜੀਉ ਪਰਿਆ ॥</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I7" s="4" t="n">
+        <v>45916.27835254629</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ਸਿਰਿ ਸਿਰਿ ਰਿਜਕੁ ਸੰਬਾਹੇ ਠਾਕੁਰੁ ਕਾਹੇ ਮਨ ਭਉ ਕਰਿਆ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਗਰਬਸਿ ਮੂੜੇ ਮਾਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>23</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਜੀਅ ਕਰਹਿ ਚਤੁਰਾਈ ॥</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ਭਾਈ ਰੇ ਭਗਤਿਹੀਣੁ ਕਾਹੇ ਜਗਿ ਆਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>32</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ਭਾਈ ਰੇ ਭਗਤਿਹੀਣੁ ਕਾਹੇ ਜਗਿ ਆਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>64</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ਸਤਿ ਕਰੇ ਜਿਨਿ ਗੁਰੂ ਪਛਾਤਾ ਸੋ ਕਾਹੇ ਕਉ ਡਰਦਾ ਜੀਉ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>101</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ਸਤਿਗੁਰੁ ਨ ਸੇਵੇ ਸੋ ਕਾਹੇ ਆਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>129</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ਸਰਨਿ ਆਵੈ ਪਾਰਬ੍ਰਹਮ ਕੀ ਤਾ ਫਿਰਿ ਕਾਹੇ ਝੂਰੇ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>132</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਬੋਲਹਿ ਜੋਗੀ ਕਪਟੁ ਘਨਾ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>156</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ਅਗਨਿ ਬਿੰਬ ਜਲ ਭੀਤਰਿ ਨਿਪਜੇ ਕਾਹੇ ਕੰਮਿ ਉਪਾਏ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>156</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ਅਬ ਢੂਢਨ ਕਾਹੇ ਕਉ ਜਾਹਿ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>178</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ਬਿਨੁ ਹਰਿ ਭਉ ਕਾਹੇ ਕਾ ਮਾਨਹਿ ॥</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>184</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ਹਰਿ ਬਿਸਰਤ ਕਾਹੇ ਸੁਖੁ ਜਾਨਹਿ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>184</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕਉ ਮੂਰਖ ਭਖਲਾਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>188</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ਗਜ ਕੋ ਤ੍ਰਾਸੁ ਮਿਟਿਓ ਜਿਹ ਸਿਮਰਤ ਤੁਮ ਕਾਹੇ ਬਿਸਰਾਵਉ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>219</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>ਮਨ ਮੂਰਖ ਕਾਹੇ ਬਿਲਲਾਈਐ ॥</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>282</v>
+      </c>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ਭੂਲਾ ਕਾਹੇ ਫਿਰਹਿ ਅਜਾਨ ॥</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>283</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਸੋਚ ਕਰਹਿ ਰੇ ਪ੍ਰਾਣੀ ॥</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>286</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ਤਬ ਲੋਗਹ ਕਾਹੇ ਦੁਖੁ ਮਾਨਿਆ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>324</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>ਤਉ ਆਨ ਬਾਟ ਕਾਹੇ ਨਹੀ ਆਇਆ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>324</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ਸੋ ਕਾਹੇ ਨ ਕਰੈ ਪ੍ਰਤਿਪਾਰ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>328</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>ਰਾਮ ਨਾਮੁ ਕਾਹੇ ਨ ਦ੍ਰਿੜ੍ਹ੍ਹੀਆ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>330</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ਤੂੰ ਸਾਜਨੁ ਸੰਗੀ ਪ੍ਰਭੁ ਮੇਰਾ ਕਾਹੇ ਜੀਅ ਡਰਾਹੀ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>378</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਏਕ ਬਿਨਾ ਚਿਤੁ ਲਾਈਐ ॥</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>379</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ਕੋਇ ਨ ਕਿਸ ਹੀ ਸੰਗਿ ਕਾਹੇ ਗਰਬੀਐ ॥</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>398</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>ਆਪੁ ਨ ਚੀਨਹਿ ਤਾਮਸੀ ਕਾਹੇ ਭਏ ਉਦਾਸਾ ॥੫॥</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>419</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>ਮਨ ਕਾਹੇ ਭੂਲੇ ਮੂੜ ਮਨਾ ॥</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>432</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>ਜਿਨੀ ਐਸਾ ਹਰਿ ਨਾਮੁ ਨ ਚੇਤਿਓ ਸੇ ਕਾਹੇ ਜਗਿ ਆਏ ਰਾਮ ਰਾਜੇ ॥</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>450</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>ਵਿਚਿ ਦੁਨੀਆ ਕਾਹੇ ਆਇਆ ॥੮॥</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>467</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਨ ਖੰਡਸਿ ਅਵਗਨੁ ਮੇਰਾ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>478</v>
+      </c>
+      <c r="F37" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>ਪ੍ਰਾਨੀ ਕਾਹੇ ਕਉ ਲੋਭਿ ਲਾਗੇ ਰਤਨ ਜਨਮੁ ਖੋਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>481</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>ਜਾ ਜਮੁ ਆਇ ਝੋਟ ਪਕਰੈ ਤਬਹਿ ਕਾਹੇ ਰੋਇਆ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>481</v>
+      </c>
+      <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>ਆਪਾ ਦੇਖਿ ਅਵਰ ਨਹੀ ਦੇਖੈ ਕਾਹੇ ਕਉ ਝਖ ਮਾਰੈ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>483</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>ਕਰਵਟੁ ਦੇ ਮੋ ਕਉ ਕਾਹੇ ਕਉ ਮਾਰੇ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>484</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕਉ ਕੀਜੈ ਧਿਆਨੁ ਜਪੰਨਾ ॥</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>485</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਰੇ ਮਨ ਚਿਤਵਹਿ ਉਦਮੁ ਜਾ ਆਹਰਿ ਹਰਿ ਜੀਉ ਪਰਿਆ ॥</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>495</v>
+      </c>
+      <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I43" s="4" t="n">
+        <v>45916.27835254629</v>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>ਸਿਰਿ ਸਿਰਿ ਰਿਜਕੁ ਸੰਬਾਹੇ ਠਾਕੁਰੁ ਕਾਹੇ ਮਨ ਭਉ ਕਰਿਆ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>495</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ਤੇਰਾ ਕੀਤਾ ਹੋਇ ਤ ਕਾਹੇ ਡਰਪੀਐ ॥</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>522</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ਹਿਰਦੈ ਕਮਲੁ ਘਟਿ ਬ੍ਰਹਮੁ ਨ ਚੀਨ੍ਹ੍ਹਾ ਕਾਹੇ ਭਇਆ ਸੰਨਿਆਸੀ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>525</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਭ੍ਰਮਤ ਹਉ ਤੁਮ ਭ੍ਰਮਹੁ ਨ ਭਾਈ ਰਵਿਆ ਰੇ ਰਵਿਆ ਸ੍ਰਬ ਥਾਨ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>535</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>ਕਾਇਆ ਕੂੜਿ ਵਿਗਾੜਿ ਕਾਹੇ ਨਾਈਐ ॥</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>565</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>ਕਾਇਆ ਕੂੜਿ ਵਿਗਾੜਿ ਕਾਹੇ ਨਾਈਐ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>566</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>ਆਗੈ ਸਰਪਰ ਜਾਣਾ ਜਿਉ ਮਿਹਮਾਣਾ ਕਾਹੇ ਗਾਰਬੁ ਕੀਜੈ ॥</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>579</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>ਜੇ ਮਨ ਜਾਣਹਿ ਸੂਲੀਆ ਕਾਹੇ ਮਿਠਾ ਖਾਹਿ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>595</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>ਰੇ ਨਰ ਕਾਹੇ ਪਪੋਰਹੁ ਦੇਹੀ ॥</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>609</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>ਦੁਖ ਹਰਤਾ ਇਹ ਬਿਧਿ ਕੋ ਸੁਆਮੀ ਤੈ ਕਾਹੇ ਬਿਸਰਾਇਆ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>632</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਭਈਆ ਫਿਰਤੌ ਫੂਲਿਆ ਫੂਲਿਆ ॥</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>654</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਰੇ ਬਨ ਖੋਜਨ ਜਾਈ ॥</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>684</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>ਰਾਮ ਨਾਮ ਛਾਡਿ ਅੰਮ੍ਰਿਤ ਕਾਹੇ ਬਿਖੁ ਖਾਈ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>692</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਰੇ ਨਰ ਗਰਬੁ ਕਰਤ ਹਹੁ ਬਿਨਸਿ ਜਾਇ ਝੂਠੀ ਦੇਹੀ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>692</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>ਏਕਾਦਸੀ ਬ੍ਰਤੁ ਰਹੈ ਕਾਹੇ ਕਉ ਤੀਰਥ ਜਾੲ​‍ਂ​‍ੀ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>718</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>ਤੂ ਕਾਹੇ ਡੋਲਹਿ ਪ੍ਰਾਣੀਆ ਤੁਧੁ ਰਾਖੈਗਾ ਸਿਰਜਣਹਾਰੁ ॥</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>724</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>ਦ੍ਵਾਰਿਕਾ ਨਗਰੀ ਕਾਹੇ ਕੇ ਮਗੋਲ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>727</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>ਅੰਮ੍ਰਿਤੁ ਛੋਡਿ ਕਾਹੇ ਬਿਖੁ ਖਾਇ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>728</v>
+      </c>
+      <c r="F61" t="b">
+        <v>1</v>
+      </c>
+      <c r="G61" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>ਸਤਿਗੁਰੁ ਸੇਵਹੁ ਆਪਨਾ ਕਾਹੇ ਫਿਰਹੁ ਅਭਾਗੇ ॥</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>809</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+      <c r="G62" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>ਦੇਖਿ ਕਸੁੰਭਾ ਰੰਗੁਲਾ ਕਾਹੇ ਭੂਲਿ ਲਾਗੇ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>809</v>
+      </c>
+      <c r="F63" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>ਅੰਤ ਕਾਲਿ ਭਜਿ ਜਾਹਿਗੇ ਕਾਹੇ ਜਲਹੁ ਕਰੋਧੀ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>809</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+      <c r="G64" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>ਐਸੇ ਕਾਹੇ ਭੂਲਿ ਪਰੇ ॥</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>823</v>
+      </c>
+      <c r="F65" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>ਜਹ ਭੀਤਰਿ ਘਟ ਭੀਤਰਿ ਬਸਿਆ ਬਾਹਰਿ ਕਾਹੇ ਨਾਹੀ ॥</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>876</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+      <c r="G66" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>ਫਿਰਿ ਫਿਰਿ ਮਾਗਨ ਕਾਹੇ ਜਾਇ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>891</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਭ੍ਰਮਿ ਭ੍ਰਮਹਿ ਬਿਗਾਨੇ ॥</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>896</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>ਸੋ ਦਾਸੁ ਅਦੇਸਾ ਕਾਹੇ ਕਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>899</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>ਪਤਿ ਵਿਣੁ ਪੂਜਾ ਸਤ ਵਿਣੁ ਸੰਜਮੁ ਜਤ ਵਿਣੁ ਕਾਹੇ ਜਨੇਊ ॥</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>903</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+      <c r="G70" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>ਆਸਣੁ ਤਿਆਗਿ ਕਾਹੇ ਸਚੁ ਪਾਵਹਿ ॥</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>903</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>ਗੁਰ ਕੀ ਕਰਣੀ ਕਾਹੇ ਧਾਵਹੁ ॥</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>933</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+      <c r="G72" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕਉ ਤੁਝੁ ਇਹੁ ਮਨੁ ਲਾਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>939</v>
+      </c>
+      <c r="F73" t="b">
+        <v>1</v>
+      </c>
+      <c r="G73" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਭੀਖਿਆ ਮੰਗਣਿ ਜਾਇ ॥੭॥</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>953</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਮਨ ਤੂ ਡੋਲਤਾ ਹਰਿ ਮਨਸਾ ਪੂਰਣਹਾਰੁ ॥</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>959</v>
+      </c>
+      <c r="F75" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਮੇਰੇ ਬਾਮ੍ਹ੍ਹਨ ਹਰਿ ਨ ਕਹਹਿ ॥</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>970</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+      <c r="G76" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>ਮੂਰਖ ਮਨ ਕਾਹੇ ਕਰਸਹਿ ਮਾਣਾ ॥</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>989</v>
+      </c>
+      <c r="F77" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>ਹਥੀ ਪਉਦੀ ਕਾਹੇ ਰੋਵੈ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>989</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>ਪ੍ਰਾਨ ਸੁਖਦਾਤਾ ਜੀਅ ਸੁਖਦਾਤਾ ਤੁਮ ਕਾਹੇ ਬਿਸਾਰਿਓ ਅਗਿਆਨਥ ॥</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>1001</v>
+      </c>
+      <c r="F79" t="b">
+        <v>1</v>
+      </c>
+      <c r="G79" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>ਅੰਦਰੁ ਖੋਜੇ ਸਬਦੁ ਸਾਲਾਹੇ ਬਾਹਰਿ ਕਾਹੇ ਜਾਹਾ ਹੇ ॥੬॥</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1056</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>ਬਹੁਰਿ ਹਮ ਕਾਹੇ ਆਵਹਿਗੇ ॥</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>1103</v>
+      </c>
+      <c r="F81" t="b">
+        <v>1</v>
+      </c>
+      <c r="G81" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀਜਤੁ ਹੈ ਮਨਿ ਭਾਵਨੁ ॥</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>1104</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+      <c r="G82" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਨ ਬਾਲਮੀਕਹਿ ਦੇਖ ॥</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>1124</v>
+      </c>
+      <c r="F83" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>ਜਿਨ ਹਰਿ ਕਾ ਨਾਮੁ ਨ ਗੁਰਮੁਖਿ ਜਾਤਾ ਸੇ ਜਗ ਮਹਿ ਕਾਹੇ ਆਇਆ ॥</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>1130</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>ਮਨੁ ਨ ਡਿਗੈ ਤਨੁ ਕਾਹੇ ਕਉ ਡਰਾਇ ॥</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>1162</v>
+      </c>
+      <c r="F85" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>ਛੀਪੇ ਕੇ ਜਨਮਿ ਕਾਹੇ ਕਉ ਆਇਆ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>1164</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕਲਰਾ ਸਿੰਚਹੁ ਜਨਮੁ ਗਵਾਵਹੁ ॥</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>1171</v>
+      </c>
+      <c r="F87" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>ਕਾਚੀ ਢਹਗਿ ਦਿਵਾਲ ਕਾਹੇ ਗਚੁ ਲਾਵਹੁ ॥੧॥ ਰਹਾਉ ॥</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>1171</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>ਮਨਮੁਖ ਭੂਲੇ ਕਾਹੇ ਆਏ ॥</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>1174</v>
+      </c>
+      <c r="F89" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਜਨਮੁ ਗਵਾਵਹੁ ਵੈਰਿ ਵਾਦਿ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>1176</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>ਮੂੜ੍ਹ੍ਹੇ ਕਾਹੇ ਬਿਸਾਰਿਓ ਤੈ ਰਾਮ ਨਾਮ ॥</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>1189</v>
+      </c>
+      <c r="F91" t="b">
+        <v>1</v>
+      </c>
+      <c r="G91" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਮਾਲੁ ਦਰਬੁ ਦੇਖਿ ਗਰਬਿ ਜਾਹਿ ॥</t>
+        </is>
+      </c>
+      <c r="E92" t="n">
+        <v>1189</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+      <c r="G92" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਪੂਤ ਝਗਰਤ ਹਉ ਸੰਗਿ ਬਾਪ ॥</t>
+        </is>
+      </c>
+      <c r="E93" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F93" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>ਰੇ ਮੂੜ੍ਹ੍ਹੇ ਆਨ ਕਾਹੇ ਕਤ ਜਾਈ ॥</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>1213</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+      <c r="G94" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>ਮੇਰੇ ਮਨ ਕਾਹੇ ਰੋਸੁ ਕਰੀਜੈ ॥</t>
+        </is>
+      </c>
+      <c r="E95" t="n">
+        <v>1262</v>
+      </c>
+      <c r="F95" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>ਏਕੋ ਕਹੀਐ ਨਾਨਕਾ ਦੂਜਾ ਕਾਹੇ ਕੂ ॥੨॥</t>
+        </is>
+      </c>
+      <c r="E96" t="n">
+        <v>1291</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>ਬਿਖੈ ਰਸ ਸਿਉ ਆਸਕਤ ਮੂੜੇ ਕਾਹੇ ਸੁਖ ਮਾਨਿ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>1303</v>
+      </c>
+      <c r="F97" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਰੇ ਮਨ ਮੋਹਿ ਮਗਨੇਰੈ ॥</t>
+        </is>
+      </c>
+      <c r="E98" t="n">
+        <v>1304</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+      <c r="G98" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>ਸੁਪਨੇ ਜਿਉ ਧਨੁ ਪਛਾਨੁ ਕਾਹੇ ਪਰਿ ਕਰਤ ਮਾਨੁ ॥</t>
+        </is>
+      </c>
+      <c r="E99" t="n">
+        <v>1352</v>
+      </c>
+      <c r="F99" t="b">
+        <v>1</v>
+      </c>
+      <c r="G99" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>ਹਰਿਚੰਦਉਰੀ ਪੇਖਿ ਕਾਹੇ ਸੁਖੁ ਮਾਨਿਆ ॥</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>1363</v>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>ਹਰਿਹਾਂ ਹਰਿਚੰਦਉਰੀ ਪੇਖਿ ਕਾਹੇ ਸਚੁ ਮਾਨਈ ॥੨੦॥</t>
+        </is>
+      </c>
+      <c r="E101" t="n">
+        <v>1363</v>
+      </c>
+      <c r="F101" t="b">
+        <v>1</v>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਛੀਪਹੁ ਛਾਇਲੈ ਰਾਮ ਨ ਲਾਵਹੁ ਚੀਤੁ ॥੨੧੨॥</t>
+        </is>
+      </c>
+      <c r="E102" t="n">
+        <v>1375</v>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ ਕੀ ਕੁਸਲਾਤ ਹਾਥਿ ਦੀਪੁ ਕੂਏ ਪਰੈ ॥੨੧੬॥</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>1376</v>
+      </c>
+      <c r="F103" t="b">
+        <v>1</v>
+      </c>
+      <c r="G103" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>ਕਬੀਰ ਕੋਠੇ ਮੰਡਪ ਹੇਤੁ ਕਰਿ ਕਾਹੇ ਮਰਹੁ ਸਵਾਰਿ ॥</t>
+        </is>
+      </c>
+      <c r="E104" t="n">
+        <v>1376</v>
+      </c>
+      <c r="F104" t="b">
+        <v>1</v>
+      </c>
+      <c r="G104" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>ਕਾਹੇ</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>ਬਿਖਿਅਨ ਸਿਉ ਕਾਹੇ ਰਚਿਓ ਨਿਮਖ ਨ ਹੋਹਿ ਉਦਾਸੁ ॥</t>
+        </is>
+      </c>
+      <c r="E105" t="n">
+        <v>1426</v>
+      </c>
+      <c r="F105" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" s="4" t="n">
+        <v>45916.27144472222</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Output files after running the script
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -608,11 +608,9 @@
         <v>45915.63580013889</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>45915.64647622685</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -847,12 +845,10 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>45915.63961045139</v>
-      </c>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Add _populate_cards_multiselect and enable multi-select verse cards in hits modal   - introduce _populate_cards_multiselect to render two-column checkbox cards with preserved centering, wraplength recalculation, and no score row while tracking selection state across pages   - expand _compute_verse_hits_for_token and refactor show_word_verse_hits_modal so verse metadata populates the new multiselect experience, keeping Select All/Clear All and pagination working with persistent selections   - in show_word_translation_input, auto-select and highlight the driver’s target word using self._word_selection_locked_vars, preventing user deselection and keeping global “Select/Deselect All” from clearing it   - verified with python -m py_compile 1.1.0_birha.py
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A2:XFD3"/>
@@ -654,6 +654,44 @@
       </c>
       <c r="L4" t="inlineStr"/>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>45920.28437333334</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -665,7 +703,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A2:XFD7"/>
@@ -4395,6 +4433,288 @@
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
     </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਪ੍ਰਾਣੀ ਪਹਿਲੈ ਪਹਰੈ ਹੁਕਮਿ ਪਇਆ ਗਰਭਾਸਿ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>74</v>
+      </c>
+      <c r="F106" t="b">
+        <v>1</v>
+      </c>
+      <c r="G106" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I106" s="4" t="n">
+        <v>45920.2914711574</v>
+      </c>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਪ੍ਰਾਣੀ ਤੀਜੈ ਪਹਰੈ ਪ੍ਰਭੁ ਚੇਤਹੁ ਲਿਵ ਲਾਇ ॥੩॥</t>
+        </is>
+      </c>
+      <c r="E107" t="n">
+        <v>76</v>
+      </c>
+      <c r="F107" t="b">
+        <v>1</v>
+      </c>
+      <c r="G107" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਜਉ ਸਾਧਸੰਗੁ ਪਾਇਓ ਤਉ ਫਿਰਿ ਜਨਮਿ ਨ ਆਵਉ ॥੪॥੧॥੧੨੧॥</t>
+        </is>
+      </c>
+      <c r="E108" t="n">
+        <v>401</v>
+      </c>
+      <c r="F108" t="b">
+        <v>1</v>
+      </c>
+      <c r="G108" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਲੋਗ ਅਲੋਗੀ ਰੀ ਸਖੀ ॥੨॥੧॥੧੫੭॥</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>409</v>
+      </c>
+      <c r="F109" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਥਿਰੁ ਕਛੁ ਨਹੀ ਸੁਪਨੇ ਜਿਉ ਸੰਸਾਰੁ ॥੫੦॥</t>
+        </is>
+      </c>
+      <c r="E110" t="n">
+        <v>1429</v>
+      </c>
+      <c r="F110" t="b">
+        <v>1</v>
+      </c>
+      <c r="G110" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਅਬ ਓਟ ਹਰਿ ਗਜ ਜਿਉ ਹੋਹੁ ਸਹਾਇ ॥੫੩॥</t>
+        </is>
+      </c>
+      <c r="E111" t="n">
+        <v>1429</v>
+      </c>
+      <c r="F111" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>45920.28428170139</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਹਮ ਨੀਚ ਕਰੰਮਾ ॥</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>12</v>
+      </c>
+      <c r="F112" t="b">
+        <v>1</v>
+      </c>
+      <c r="G112" s="4" t="n">
+        <v>45920.30639990741</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>ਕਹੁ</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>ਕਹੁ ਨਾਨਕ ਪ੍ਰਾਣੀ ਪਹਿਲੈ ਪਹਰੈ ਛੂਟਹਿਗਾ ਹਰਿ ਚੇਤਿ ॥੧॥</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>75</v>
+      </c>
+      <c r="F113" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>45920.30639990741</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>not started</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Auto-select + highlight derived grammar suggestions and refresh after each CSV save   - add a derived-suggestion cache with mtime reloads and Derived-only dominance logic so Number/Gender/Type defaults stay current   - auto-select and highlight dominant radio options in _build_user_input_grammar, keeping Tk traces in sync after cache invalidation   - clear suggestion cache whenever _append_birha_csv_row overwrites or appends so new Derived rows surface immediately
  Tests: python -m py_compile 1.1.0_birha.py
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -684,9 +684,11 @@
         <v>45920.28437333334</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>45921.26947563657</v>
+      </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
@@ -1029,10 +1031,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>45921.26109167824</v>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
     </row>
@@ -2291,10 +2295,12 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I44" s="4" t="n">
+        <v>45921.26109167824</v>
+      </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
     </row>
@@ -4498,10 +4504,12 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I107" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I107" s="4" t="n">
+        <v>45921.26947415509</v>
+      </c>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
     </row>
@@ -4533,10 +4541,12 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I108" s="4" t="n">
+        <v>45921.26443756944</v>
+      </c>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
     </row>
@@ -4568,10 +4578,12 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I109" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I109" s="4" t="n">
+        <v>45921.26574731481</v>
+      </c>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
     </row>
@@ -4603,10 +4615,12 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I110" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I110" s="4" t="n">
+        <v>45921.26642972222</v>
+      </c>
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
     </row>
@@ -4638,10 +4652,12 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I111" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I111" s="4" t="n">
+        <v>45921.26742945602</v>
+      </c>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
     </row>
@@ -4673,10 +4689,12 @@
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I112" s="4" t="n">
+        <v>45921.26840819445</v>
+      </c>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
     </row>
@@ -4708,10 +4726,12 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I113" s="4" t="n">
+        <v>45921.26889071759</v>
+      </c>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
Update to output files
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -608,9 +608,11 @@
         <v>45915.63580013889</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="n">
+        <v>45921.45275196759</v>
+      </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
@@ -705,7 +707,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A2:XFD7"/>
@@ -782,6 +784,31 @@
           <t>last_reanalyzed_at</t>
         </is>
       </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>removed_at</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>archived_at</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>superseded_at</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>verse_key_norm</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -819,6 +846,11 @@
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -856,6 +888,11 @@
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -885,12 +922,21 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>not started</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>45921.45275030092</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -928,6 +974,11 @@
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -965,6 +1016,11 @@
       </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1002,6 +1058,11 @@
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1039,6 +1100,11 @@
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1074,6 +1140,11 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1109,6 +1180,11 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1144,6 +1220,11 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1179,6 +1260,11 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1214,6 +1300,11 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1249,6 +1340,11 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1284,6 +1380,11 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1319,6 +1420,11 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1341,19 +1447,26 @@
         <v>156</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="4" t="n">
         <v>45916.27144472222</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>not started</t>
+          <t>removed</t>
         </is>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" s="4" t="n">
+        <v>45921.45078101852</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1389,6 +1502,11 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1424,6 +1542,11 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1459,6 +1582,11 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1494,6 +1622,11 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1529,6 +1662,11 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1564,6 +1702,11 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1599,6 +1742,11 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1634,6 +1782,11 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1669,6 +1822,11 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1704,6 +1862,11 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1739,6 +1902,11 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1774,6 +1942,11 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1809,6 +1982,11 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1844,6 +2022,11 @@
       <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1879,6 +2062,11 @@
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1914,6 +2102,11 @@
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1949,6 +2142,11 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1984,6 +2182,11 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2019,6 +2222,11 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2054,6 +2262,11 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2089,6 +2302,11 @@
       <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2124,6 +2342,11 @@
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2159,6 +2382,11 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2194,6 +2422,11 @@
       <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2229,6 +2462,11 @@
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2266,6 +2504,11 @@
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2303,6 +2546,11 @@
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2338,6 +2586,11 @@
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2373,6 +2626,11 @@
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2408,6 +2666,11 @@
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2443,6 +2706,11 @@
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2478,6 +2746,11 @@
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2513,6 +2786,11 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2548,6 +2826,11 @@
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2583,6 +2866,11 @@
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr"/>
       <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2618,6 +2906,11 @@
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2653,6 +2946,11 @@
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2688,6 +2986,11 @@
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2723,6 +3026,11 @@
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr"/>
       <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2758,6 +3066,11 @@
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2793,6 +3106,11 @@
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2828,6 +3146,11 @@
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr"/>
       <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2863,6 +3186,11 @@
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2898,6 +3226,11 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2933,6 +3266,11 @@
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2968,6 +3306,11 @@
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3003,6 +3346,11 @@
       <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr"/>
       <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3038,6 +3386,11 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3073,6 +3426,11 @@
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3108,6 +3466,11 @@
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr"/>
       <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3143,6 +3506,11 @@
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr"/>
       <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3178,6 +3546,11 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3213,6 +3586,11 @@
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3248,6 +3626,11 @@
       <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr"/>
       <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3283,6 +3666,11 @@
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr"/>
       <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3318,6 +3706,11 @@
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3353,6 +3746,11 @@
       <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3388,6 +3786,11 @@
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3423,6 +3826,11 @@
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3458,6 +3866,11 @@
       <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr"/>
       <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3493,6 +3906,11 @@
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3528,6 +3946,11 @@
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3563,6 +3986,11 @@
       <c r="I80" t="inlineStr"/>
       <c r="J80" t="inlineStr"/>
       <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3598,6 +4026,11 @@
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3633,6 +4066,11 @@
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3668,6 +4106,11 @@
       <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3703,6 +4146,11 @@
       <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr"/>
       <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3738,6 +4186,11 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3773,6 +4226,11 @@
       <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr"/>
       <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3808,6 +4266,11 @@
       <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr"/>
       <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3843,6 +4306,11 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3878,6 +4346,11 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3913,6 +4386,11 @@
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3948,6 +4426,11 @@
       <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3983,6 +4466,11 @@
       <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4018,6 +4506,11 @@
       <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr"/>
       <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4053,6 +4546,11 @@
       <c r="I94" t="inlineStr"/>
       <c r="J94" t="inlineStr"/>
       <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4088,6 +4586,11 @@
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4123,6 +4626,11 @@
       <c r="I96" t="inlineStr"/>
       <c r="J96" t="inlineStr"/>
       <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4158,6 +4666,11 @@
       <c r="I97" t="inlineStr"/>
       <c r="J97" t="inlineStr"/>
       <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4193,6 +4706,11 @@
       <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr"/>
       <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4228,6 +4746,11 @@
       <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr"/>
       <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4263,6 +4786,11 @@
       <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr"/>
       <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4298,6 +4826,11 @@
       <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4333,6 +4866,11 @@
       <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr"/>
       <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4368,6 +4906,11 @@
       <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr"/>
       <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4403,6 +4946,11 @@
       <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr"/>
       <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4438,6 +4986,11 @@
       <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr"/>
       <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4475,6 +5028,11 @@
       </c>
       <c r="J106" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4512,6 +5070,11 @@
       </c>
       <c r="J107" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4549,6 +5112,11 @@
       </c>
       <c r="J108" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4586,6 +5154,11 @@
       </c>
       <c r="J109" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4623,6 +5196,11 @@
       </c>
       <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4660,6 +5238,11 @@
       </c>
       <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4697,6 +5280,11 @@
       </c>
       <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4734,6 +5322,11 @@
       </c>
       <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Maximise buttons added to dialogs
</commit_message>
<xml_diff>
--- a/1.1.6_assess_by_word.xlsx
+++ b/1.1.6_assess_by_word.xlsx
@@ -1092,7 +1092,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>completed</t>
+          <t>archived</t>
         </is>
       </c>
       <c r="I8" s="4" t="n">
@@ -1102,7 +1102,9 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" s="4" t="n">
+        <v>45922.40734116898</v>
+      </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
     </row>
@@ -2538,7 +2540,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>completed</t>
+          <t>archived</t>
         </is>
       </c>
       <c r="I44" s="4" t="n">
@@ -2548,7 +2550,9 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
+      <c r="N44" s="4" t="n">
+        <v>45922.40742258102</v>
+      </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
     </row>

</xml_diff>